<commit_message>
Updated to Serie A Round 22
</commit_message>
<xml_diff>
--- a/leagueStats/leagueStats_ITA_full.xlsx
+++ b/leagueStats/leagueStats_ITA_full.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O209"/>
+  <dimension ref="A1:O219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11113,6 +11113,516 @@
         <v>4</v>
       </c>
     </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>2</v>
+      </c>
+      <c r="E210" t="n">
+        <v>0</v>
+      </c>
+      <c r="F210" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="G210" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="H210" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="I210" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="J210" t="n">
+        <v>0</v>
+      </c>
+      <c r="K210" t="n">
+        <v>0</v>
+      </c>
+      <c r="L210" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M210" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="N210" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="O210" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>1</v>
+      </c>
+      <c r="E211" t="n">
+        <v>2</v>
+      </c>
+      <c r="F211" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G211" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H211" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="I211" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J211" t="n">
+        <v>0</v>
+      </c>
+      <c r="K211" t="n">
+        <v>0</v>
+      </c>
+      <c r="L211" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="M211" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N211" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O211" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>1</v>
+      </c>
+      <c r="E212" t="n">
+        <v>1</v>
+      </c>
+      <c r="F212" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G212" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H212" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="I212" t="n">
+        <v>1</v>
+      </c>
+      <c r="J212" t="n">
+        <v>1</v>
+      </c>
+      <c r="K212" t="n">
+        <v>0</v>
+      </c>
+      <c r="L212" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="M212" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="N212" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="O212" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>2</v>
+      </c>
+      <c r="E213" t="n">
+        <v>1</v>
+      </c>
+      <c r="F213" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="G213" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="H213" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="I213" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J213" t="n">
+        <v>2</v>
+      </c>
+      <c r="K213" t="n">
+        <v>0</v>
+      </c>
+      <c r="L213" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="M213" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="N213" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="O213" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>1</v>
+      </c>
+      <c r="E214" t="n">
+        <v>2</v>
+      </c>
+      <c r="F214" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="G214" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="H214" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="I214" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J214" t="n">
+        <v>0</v>
+      </c>
+      <c r="K214" t="n">
+        <v>0</v>
+      </c>
+      <c r="L214" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M214" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N214" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="O214" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>0</v>
+      </c>
+      <c r="E215" t="n">
+        <v>4</v>
+      </c>
+      <c r="F215" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G215" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="H215" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="I215" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="J215" t="n">
+        <v>0</v>
+      </c>
+      <c r="K215" t="n">
+        <v>1</v>
+      </c>
+      <c r="L215" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M215" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="N215" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="O215" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>3</v>
+      </c>
+      <c r="E216" t="n">
+        <v>2</v>
+      </c>
+      <c r="F216" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="G216" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="H216" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="I216" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="J216" t="n">
+        <v>2</v>
+      </c>
+      <c r="K216" t="n">
+        <v>0</v>
+      </c>
+      <c r="L216" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M216" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="N216" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O216" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>1</v>
+      </c>
+      <c r="E217" t="n">
+        <v>2</v>
+      </c>
+      <c r="F217" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G217" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="H217" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="I217" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="J217" t="n">
+        <v>0</v>
+      </c>
+      <c r="K217" t="n">
+        <v>2</v>
+      </c>
+      <c r="L217" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="M217" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="N217" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="O217" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="D218" t="n">
+        <v>2</v>
+      </c>
+      <c r="E218" t="n">
+        <v>0</v>
+      </c>
+      <c r="F218" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="G218" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H218" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="I218" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="J218" t="n">
+        <v>1</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0</v>
+      </c>
+      <c r="L218" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M218" t="n">
+        <v>0</v>
+      </c>
+      <c r="N218" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="O218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>1</v>
+      </c>
+      <c r="E219" t="n">
+        <v>1</v>
+      </c>
+      <c r="F219" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="G219" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="H219" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="I219" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="J219" t="n">
+        <v>0</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M219" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="N219" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="O219" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>